<commit_message>
Added references to all locations.
</commit_message>
<xml_diff>
--- a/src/data/a-record-of-buddhistic-kingdoms.xlsx
+++ b/src/data/a-record-of-buddhistic-kingdoms.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2244" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2304" uniqueCount="628">
   <si>
     <t>Google Maps</t>
   </si>
@@ -3113,6 +3113,15 @@
       <c r="AM9" s="2">
         <v>2.0</v>
       </c>
+      <c r="AN9" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO9" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP9" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
@@ -3157,6 +3166,15 @@
       <c r="AM10" s="2">
         <v>2.0</v>
       </c>
+      <c r="AN10" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO10" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="AP10" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -3201,6 +3219,15 @@
       <c r="AM11" s="2">
         <v>2.0</v>
       </c>
+      <c r="AN11" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO11" s="2">
+        <v>13.0</v>
+      </c>
+      <c r="AP11" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AQ11" s="2">
         <v>99.0</v>
       </c>
@@ -3240,6 +3267,15 @@
       <c r="AM12" s="2">
         <v>4.0</v>
       </c>
+      <c r="AN12" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO12" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AP12" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
@@ -3269,6 +3305,15 @@
       <c r="AM13" s="2">
         <v>4.0</v>
       </c>
+      <c r="AN13" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO13" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="AP13" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
@@ -3298,6 +3343,15 @@
       <c r="AM14" s="2">
         <v>4.0</v>
       </c>
+      <c r="AN14" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO14" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="AP14" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
@@ -3327,6 +3381,15 @@
       <c r="AM15" s="2">
         <v>6.0</v>
       </c>
+      <c r="AN15" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO15" s="2">
+        <v>5.0</v>
+      </c>
+      <c r="AP15" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
@@ -3356,6 +3419,15 @@
       <c r="AM16" s="2">
         <v>8.0</v>
       </c>
+      <c r="AN16" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO16" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP16" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
@@ -3385,6 +3457,15 @@
       <c r="AM17" s="2">
         <v>8.0</v>
       </c>
+      <c r="AN17" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AO17" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AP17" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
@@ -3414,6 +3495,15 @@
       <c r="AM18" s="2">
         <v>10.0</v>
       </c>
+      <c r="AN18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO18" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
@@ -3443,6 +3533,15 @@
       <c r="AM19" s="2">
         <v>11.0</v>
       </c>
+      <c r="AN19" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO19" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP19" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
@@ -3472,6 +3571,15 @@
       <c r="AM20" s="2">
         <v>12.0</v>
       </c>
+      <c r="AN20" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO20" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP20" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="s">
@@ -3510,6 +3618,15 @@
       <c r="AM21" s="2">
         <v>13.0</v>
       </c>
+      <c r="AN21" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO21" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP21" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AQ21" s="2">
         <v>30.0</v>
       </c>
@@ -3552,6 +3669,15 @@
       <c r="AM22" s="2">
         <v>13.0</v>
       </c>
+      <c r="AN22" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AO22" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP22" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AQ22" s="2">
         <v>30.0</v>
       </c>
@@ -3594,6 +3720,15 @@
       <c r="AM23" s="2">
         <v>13.0</v>
       </c>
+      <c r="AN23" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AO23" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP23" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AQ23" s="2">
         <v>30.0</v>
       </c>
@@ -3876,6 +4011,15 @@
       <c r="AM27" s="2">
         <v>15.0</v>
       </c>
+      <c r="AN27" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO27" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP27" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="s">
@@ -3905,6 +4049,15 @@
       <c r="AM28" s="2">
         <v>16.0</v>
       </c>
+      <c r="AN28" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO28" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AP28" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="s">
@@ -3934,6 +4087,15 @@
       <c r="AM29" s="2">
         <v>17.0</v>
       </c>
+      <c r="AN29" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO29" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP29" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="s">
@@ -3963,6 +4125,15 @@
       <c r="AM30" s="2">
         <v>18.0</v>
       </c>
+      <c r="AN30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO30" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP30" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="s">
@@ -3992,6 +4163,15 @@
       <c r="AM31" s="2">
         <v>18.0</v>
       </c>
+      <c r="AN31" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AO31" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP31" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
@@ -4021,6 +4201,15 @@
       <c r="AM32" s="2">
         <v>19.0</v>
       </c>
+      <c r="AN32" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO32" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP32" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="s">
@@ -4053,6 +4242,15 @@
       <c r="AM33" s="2">
         <v>20.0</v>
       </c>
+      <c r="AN33" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO33" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP33" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="s">
@@ -4082,6 +4280,15 @@
       <c r="AM34" s="2">
         <v>21.0</v>
       </c>
+      <c r="AN34" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO34" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP34" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="s">
@@ -4111,6 +4318,15 @@
       <c r="AM35" s="2">
         <v>21.0</v>
       </c>
+      <c r="AN35" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AO35" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP35" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="s">
@@ -4140,6 +4356,15 @@
       <c r="AM36" s="2">
         <v>21.0</v>
       </c>
+      <c r="AN36" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AO36" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AP36" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="s">
@@ -4169,6 +4394,15 @@
       <c r="AM37" s="2">
         <v>22.0</v>
       </c>
+      <c r="AN37" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO37" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP37" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AQ37" s="2">
         <v>99.0</v>
       </c>
@@ -4202,6 +4436,15 @@
       <c r="AM38" s="2">
         <v>22.0</v>
       </c>
+      <c r="AN38" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AO38" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP38" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AQ38" s="2">
         <v>99.0</v>
       </c>
@@ -4235,6 +4478,15 @@
       <c r="AM39" s="2">
         <v>23.0</v>
       </c>
+      <c r="AN39" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO39" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP39" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="s">
@@ -4264,6 +4516,15 @@
       <c r="AM40" s="2">
         <v>24.0</v>
       </c>
+      <c r="AN40" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO40" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP40" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
@@ -4296,6 +4557,15 @@
       <c r="AM41" s="2">
         <v>24.0</v>
       </c>
+      <c r="AN41" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AO41" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP41" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AQ41" s="2">
         <v>90.0</v>
       </c>
@@ -4329,6 +4599,15 @@
       <c r="AM42" s="2">
         <v>24.0</v>
       </c>
+      <c r="AN42" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AO42" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP42" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
@@ -4361,6 +4640,15 @@
       <c r="AM43" s="2">
         <v>24.0</v>
       </c>
+      <c r="AN43" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="AO43" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AP43" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="s">
@@ -4390,6 +4678,15 @@
       <c r="AM44" s="2">
         <v>25.0</v>
       </c>
+      <c r="AN44" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO44" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP44" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="s">
@@ -4419,6 +4716,15 @@
       <c r="AM45" s="2">
         <v>25.0</v>
       </c>
+      <c r="AN45" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AO45" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP45" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="s">
@@ -4570,6 +4876,15 @@
       <c r="AM47" s="2">
         <v>27.0</v>
       </c>
+      <c r="AN47" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO47" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP47" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="s">
@@ -4599,6 +4914,15 @@
       <c r="AM48" s="2">
         <v>27.0</v>
       </c>
+      <c r="AN48" s="2">
+        <v>6.0</v>
+      </c>
+      <c r="AO48" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="AP48" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="s">
@@ -4628,6 +4952,15 @@
       <c r="AM49" s="2">
         <v>28.0</v>
       </c>
+      <c r="AN49" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO49" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP49" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
@@ -4657,6 +4990,15 @@
       <c r="AM50" s="2">
         <v>28.0</v>
       </c>
+      <c r="AN50" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AO50" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP50" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="s">
@@ -4689,6 +5031,15 @@
       <c r="AM51" s="2">
         <v>28.0</v>
       </c>
+      <c r="AN51" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AO51" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP51" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
@@ -4718,6 +5069,15 @@
       <c r="AM52" s="2">
         <v>29.0</v>
       </c>
+      <c r="AN52" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO52" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP52" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="s">
@@ -4753,6 +5113,15 @@
       <c r="AM53" s="2">
         <v>29.0</v>
       </c>
+      <c r="AN53" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO53" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AP53" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="s">
@@ -4788,6 +5157,15 @@
       <c r="AM54" s="2">
         <v>29.0</v>
       </c>
+      <c r="AN54" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO54" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AP54" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="s">
@@ -4867,6 +5245,15 @@
       <c r="AM56" s="2">
         <v>30.0</v>
       </c>
+      <c r="AN56" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO56" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP56" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="s">
@@ -4896,6 +5283,15 @@
       <c r="AM57" s="2">
         <v>30.0</v>
       </c>
+      <c r="AN57" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AO57" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP57" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="s">
@@ -4928,6 +5324,15 @@
       <c r="AM58" s="2">
         <v>30.0</v>
       </c>
+      <c r="AN58" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AO58" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP58" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
@@ -4957,6 +5362,15 @@
       <c r="AM59" s="2">
         <v>30.0</v>
       </c>
+      <c r="AN59" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="AO59" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP59" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="1" t="s">
@@ -5030,6 +5444,15 @@
       <c r="AM61" s="2">
         <v>31.0</v>
       </c>
+      <c r="AN61" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO61" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP61" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AQ61" s="2">
         <v>99.0</v>
       </c>
@@ -5063,6 +5486,15 @@
       <c r="AM62" s="2">
         <v>31.0</v>
       </c>
+      <c r="AN62" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO62" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AP62" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="AQ62" s="2">
         <v>99.0</v>
       </c>
@@ -5096,6 +5528,15 @@
       <c r="AM63" s="2">
         <v>33.0</v>
       </c>
+      <c r="AN63" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO63" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP63" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="s">
@@ -5125,6 +5566,15 @@
       <c r="AM64" s="2">
         <v>34.0</v>
       </c>
+      <c r="AN64" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO64" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP64" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="s">
@@ -5151,6 +5601,15 @@
       <c r="AM65" s="2">
         <v>34.0</v>
       </c>
+      <c r="AN65" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO65" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AP65" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="1" t="s">
@@ -5180,6 +5639,15 @@
       <c r="AM66" s="2">
         <v>34.0</v>
       </c>
+      <c r="AN66" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AO66" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP66" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="1" t="s">
@@ -5206,6 +5674,15 @@
       <c r="AM67" s="2">
         <v>34.0</v>
       </c>
+      <c r="AN67" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AO67" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AP67" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="1" t="s">
@@ -5235,6 +5712,15 @@
       <c r="AM68" s="2">
         <v>34.0</v>
       </c>
+      <c r="AN68" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="AO68" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="AP68" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="1" t="s">
@@ -5270,6 +5756,15 @@
       <c r="AM69" s="2">
         <v>34.0</v>
       </c>
+      <c r="AN69" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="AO69" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP69" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="1" t="s">
@@ -5345,6 +5840,15 @@
       <c r="AM71" s="2">
         <v>37.0</v>
       </c>
+      <c r="AN71" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO71" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP71" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="1" t="s">
@@ -5380,6 +5884,15 @@
       <c r="AM72" s="2">
         <v>37.0</v>
       </c>
+      <c r="AN72" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AO72" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AP72" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="1" t="s">
@@ -5421,6 +5934,15 @@
       <c r="AM73" s="2">
         <v>38.0</v>
       </c>
+      <c r="AN73" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AO73" s="2">
+        <v>2.0</v>
+      </c>
+      <c r="AP73" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="1" t="s">
@@ -5456,6 +5978,15 @@
       <c r="AM74" s="2">
         <v>38.0</v>
       </c>
+      <c r="AN74" s="2">
+        <v>8.0</v>
+      </c>
+      <c r="AO74" s="2">
+        <v>0.0</v>
+      </c>
+      <c r="AP74" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="1" t="s">
@@ -5688,6 +6219,15 @@
       </c>
       <c r="AM78" s="2">
         <v>40.0</v>
+      </c>
+      <c r="AN78" s="2">
+        <v>4.0</v>
+      </c>
+      <c r="AO78" s="2">
+        <v>3.0</v>
+      </c>
+      <c r="AP78" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="AQ78" s="2">
         <v>99.0</v>

</xml_diff>